<commit_message>
added write_partial_takes and write_participation
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesc/Desktop/Francesc/No_UNI/Programació/Media Arts Studio/guio_a_grafic/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34913D7-84F0-1649-861D-698AC6B7CD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBAAE3A-897C-6E4F-818A-5CE99EC3CC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" tabRatio="398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1436,7 +1436,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4361,7 +4361,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="BB8" sqref="BB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4710,154 +4710,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7286,7 +7286,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="BB7" sqref="BB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7635,154 +7635,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>134</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>141</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10211,7 +10211,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="BB8" sqref="BB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10560,154 +10560,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>154</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>156</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>157</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>167</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>169</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>172</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>173</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>179</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>181</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>182</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>183</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>184</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>186</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>187</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>188</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>191</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>192</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>193</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>195</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>197</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13136,7 +13136,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="BB7" sqref="BB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13485,154 +13485,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>202</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>203</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>206</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>211</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>212</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>216</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>218</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>219</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>221</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>222</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>224</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>225</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>227</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>228</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>229</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>231</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>232</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>233</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>234</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>235</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>236</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>237</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>238</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>239</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>241</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>242</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>244</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>246</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>247</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>248</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>249</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16061,7 +16061,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="BB7" sqref="BB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16410,154 +16410,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>251</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>252</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>253</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>254</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>255</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>256</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>257</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>258</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>259</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>260</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>261</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>262</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>264</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>265</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>266</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>267</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>268</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>269</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>270</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>271</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>272</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>273</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>274</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>275</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>276</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>277</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>278</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>279</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>280</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>281</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>282</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>283</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>284</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>285</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>286</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>287</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>288</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>289</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>290</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>291</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>292</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>293</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>294</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>296</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>297</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>299</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18986,7 +18986,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="AX18" sqref="AX18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19335,154 +19335,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>302</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>303</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>304</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>305</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>306</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>307</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>308</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>309</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>310</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>311</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>312</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>313</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>314</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>315</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>316</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>317</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>319</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>321</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>322</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>323</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>324</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>325</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>326</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>327</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>328</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>329</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>330</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>331</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>332</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>333</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>334</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>335</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>336</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>337</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>338</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>339</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>341</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>342</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>343</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>344</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>345</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>346</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>347</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>348</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>349</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21911,7 +21911,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22260,154 +22260,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>351</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>352</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>353</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>354</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>355</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>356</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>357</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>358</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>359</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>360</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>361</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>362</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>363</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>364</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>365</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>366</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>367</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>368</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>369</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>370</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>371</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>372</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>373</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>374</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>375</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>376</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>377</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>378</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>379</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>380</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>381</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>382</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>383</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>384</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>385</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>386</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>387</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>388</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>389</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>390</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>391</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>392</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>393</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>394</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>395</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>396</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>397</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>398</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>399</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24836,7 +24836,7 @@
   <dimension ref="A1:BB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25185,154 +25185,154 @@
         <v>7</v>
       </c>
       <c r="E7" s="23">
-        <v>1</v>
+        <v>401</v>
       </c>
       <c r="F7" s="23">
-        <v>2</v>
+        <v>402</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>403</v>
       </c>
       <c r="H7" s="23">
-        <v>4</v>
+        <v>404</v>
       </c>
       <c r="I7" s="23">
-        <v>5</v>
+        <v>405</v>
       </c>
       <c r="J7" s="23">
-        <v>6</v>
+        <v>406</v>
       </c>
       <c r="K7" s="23">
-        <v>7</v>
+        <v>407</v>
       </c>
       <c r="L7" s="23">
-        <v>8</v>
+        <v>408</v>
       </c>
       <c r="M7" s="23">
-        <v>9</v>
+        <v>409</v>
       </c>
       <c r="N7" s="23">
-        <v>10</v>
+        <v>410</v>
       </c>
       <c r="O7" s="23">
-        <v>11</v>
+        <v>411</v>
       </c>
       <c r="P7" s="23">
-        <v>12</v>
+        <v>412</v>
       </c>
       <c r="Q7" s="23">
-        <v>13</v>
+        <v>413</v>
       </c>
       <c r="R7" s="23">
-        <v>14</v>
+        <v>414</v>
       </c>
       <c r="S7" s="23">
-        <v>15</v>
+        <v>415</v>
       </c>
       <c r="T7" s="23">
-        <v>16</v>
+        <v>416</v>
       </c>
       <c r="U7" s="23">
-        <v>17</v>
+        <v>417</v>
       </c>
       <c r="V7" s="23">
-        <v>18</v>
+        <v>418</v>
       </c>
       <c r="W7" s="23">
-        <v>19</v>
+        <v>419</v>
       </c>
       <c r="X7" s="23">
-        <v>20</v>
+        <v>420</v>
       </c>
       <c r="Y7" s="23">
-        <v>21</v>
+        <v>421</v>
       </c>
       <c r="Z7" s="23">
-        <v>22</v>
+        <v>422</v>
       </c>
       <c r="AA7" s="23">
-        <v>23</v>
+        <v>423</v>
       </c>
       <c r="AB7" s="23">
-        <v>24</v>
+        <v>424</v>
       </c>
       <c r="AC7" s="23">
-        <v>25</v>
+        <v>425</v>
       </c>
       <c r="AD7" s="23">
-        <v>26</v>
+        <v>426</v>
       </c>
       <c r="AE7" s="23">
-        <v>27</v>
+        <v>427</v>
       </c>
       <c r="AF7" s="23">
-        <v>28</v>
+        <v>428</v>
       </c>
       <c r="AG7" s="23">
-        <v>29</v>
+        <v>429</v>
       </c>
       <c r="AH7" s="23">
-        <v>30</v>
+        <v>430</v>
       </c>
       <c r="AI7" s="23">
-        <v>31</v>
+        <v>431</v>
       </c>
       <c r="AJ7" s="23">
-        <v>32</v>
+        <v>432</v>
       </c>
       <c r="AK7" s="23">
-        <v>33</v>
+        <v>433</v>
       </c>
       <c r="AL7" s="23">
-        <v>34</v>
+        <v>434</v>
       </c>
       <c r="AM7" s="23">
-        <v>35</v>
+        <v>435</v>
       </c>
       <c r="AN7" s="23">
-        <v>36</v>
+        <v>436</v>
       </c>
       <c r="AO7" s="23">
-        <v>37</v>
+        <v>437</v>
       </c>
       <c r="AP7" s="23">
-        <v>38</v>
+        <v>438</v>
       </c>
       <c r="AQ7" s="23">
-        <v>39</v>
+        <v>439</v>
       </c>
       <c r="AR7" s="23">
-        <v>40</v>
+        <v>440</v>
       </c>
       <c r="AS7" s="23">
-        <v>41</v>
+        <v>441</v>
       </c>
       <c r="AT7" s="23">
-        <v>42</v>
+        <v>442</v>
       </c>
       <c r="AU7" s="23">
-        <v>43</v>
+        <v>443</v>
       </c>
       <c r="AV7" s="23">
-        <v>44</v>
+        <v>444</v>
       </c>
       <c r="AW7" s="23">
-        <v>45</v>
+        <v>445</v>
       </c>
       <c r="AX7" s="23">
-        <v>46</v>
+        <v>446</v>
       </c>
       <c r="AY7" s="23">
-        <v>47</v>
+        <v>447</v>
       </c>
       <c r="AZ7" s="23">
-        <v>48</v>
+        <v>448</v>
       </c>
       <c r="BA7" s="23">
-        <v>49</v>
+        <v>449</v>
       </c>
       <c r="BB7" s="31">
-        <v>50</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>